<commit_message>
updated to add farmer and delete farmer
</commit_message>
<xml_diff>
--- a/API/foodDetails.xlsx
+++ b/API/foodDetails.xlsx
@@ -8,19 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\FarmersApp\API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D39506-42DF-450B-A13D-1779F6CD12E4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0108B894-742D-4C70-BA23-200793A60E28}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15585" yWindow="-15945" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="food" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="406">
   <si>
     <t>tfvname</t>
   </si>
@@ -1235,6 +1242,9 @@
   </si>
   <si>
     <t>http://tropicalfruitandveg.com/thumb.php?image=images/arbiplant.jpg</t>
+  </si>
+  <si>
+    <t>price</t>
   </si>
 </sst>
 </file>
@@ -1574,15 +1584,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E103" sqref="E103:E132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1595,8 +1605,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1609,8 +1622,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1623,8 +1639,11 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>2.84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1637,8 +1656,11 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>8.2799999999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1651,8 +1673,11 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1665,8 +1690,11 @@
       <c r="D6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>6.92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1679,8 +1707,11 @@
       <c r="D7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1693,8 +1724,11 @@
       <c r="D8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1707,8 +1741,11 @@
       <c r="D9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>4.76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1721,8 +1758,11 @@
       <c r="D10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1735,8 +1775,11 @@
       <c r="D11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>6.81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1749,8 +1792,11 @@
       <c r="D12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>3.07</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1763,8 +1809,11 @@
       <c r="D13" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>5.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1777,8 +1826,11 @@
       <c r="D14" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -1791,8 +1843,11 @@
       <c r="D15" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -1805,8 +1860,11 @@
       <c r="D16" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>8.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>62</v>
       </c>
@@ -1819,8 +1877,11 @@
       <c r="D17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>4.5199999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -1833,8 +1894,11 @@
       <c r="D18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>6.22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -1847,8 +1911,11 @@
       <c r="D19" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -1861,8 +1928,11 @@
       <c r="D20" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -1875,8 +1945,11 @@
       <c r="D21" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>5.44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -1889,8 +1962,11 @@
       <c r="D22" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>86</v>
       </c>
@@ -1903,8 +1979,11 @@
       <c r="D23" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>90</v>
       </c>
@@ -1917,8 +1996,11 @@
       <c r="D24" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>6.89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -1931,8 +2013,11 @@
       <c r="D25" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -1945,8 +2030,11 @@
       <c r="D26" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>9.77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>102</v>
       </c>
@@ -1959,8 +2047,11 @@
       <c r="D27" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>6.27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>106</v>
       </c>
@@ -1973,8 +2064,11 @@
       <c r="D28" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>110</v>
       </c>
@@ -1987,8 +2081,11 @@
       <c r="D29" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>114</v>
       </c>
@@ -2001,8 +2098,11 @@
       <c r="D30" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>2.63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>118</v>
       </c>
@@ -2015,8 +2115,11 @@
       <c r="D31" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>5.76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>122</v>
       </c>
@@ -2029,8 +2132,11 @@
       <c r="D32" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>3.61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>126</v>
       </c>
@@ -2043,8 +2149,11 @@
       <c r="D33" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>5.46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>130</v>
       </c>
@@ -2057,8 +2166,11 @@
       <c r="D34" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>134</v>
       </c>
@@ -2071,8 +2183,11 @@
       <c r="D35" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>5.59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>138</v>
       </c>
@@ -2085,8 +2200,11 @@
       <c r="D36" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -2099,8 +2217,11 @@
       <c r="D37" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>146</v>
       </c>
@@ -2113,8 +2234,11 @@
       <c r="D38" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>150</v>
       </c>
@@ -2127,8 +2251,11 @@
       <c r="D39" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>8.85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>154</v>
       </c>
@@ -2141,8 +2268,11 @@
       <c r="D40" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>7.41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>158</v>
       </c>
@@ -2155,8 +2285,11 @@
       <c r="D41" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>9.23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>162</v>
       </c>
@@ -2169,8 +2302,11 @@
       <c r="D42" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>6.09</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>166</v>
       </c>
@@ -2183,8 +2319,11 @@
       <c r="D43" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>8.89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>170</v>
       </c>
@@ -2197,8 +2336,11 @@
       <c r="D44" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>8.81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>174</v>
       </c>
@@ -2211,8 +2353,11 @@
       <c r="D45" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>178</v>
       </c>
@@ -2225,8 +2370,11 @@
       <c r="D46" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>182</v>
       </c>
@@ -2239,8 +2387,11 @@
       <c r="D47" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>9.66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>186</v>
       </c>
@@ -2253,8 +2404,11 @@
       <c r="D48" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>3.54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>190</v>
       </c>
@@ -2267,8 +2421,11 @@
       <c r="D49" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>8.4499999999999993</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>194</v>
       </c>
@@ -2281,8 +2438,11 @@
       <c r="D50" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>9.9700000000000006</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>198</v>
       </c>
@@ -2295,8 +2455,11 @@
       <c r="D51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>202</v>
       </c>
@@ -2309,8 +2472,11 @@
       <c r="D52" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>6.26</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>206</v>
       </c>
@@ -2323,8 +2489,11 @@
       <c r="D53" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>9.94</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>210</v>
       </c>
@@ -2337,8 +2506,11 @@
       <c r="D54" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>214</v>
       </c>
@@ -2351,8 +2523,11 @@
       <c r="D55" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>5.82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>218</v>
       </c>
@@ -2365,8 +2540,11 @@
       <c r="D56" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>222</v>
       </c>
@@ -2379,8 +2557,11 @@
       <c r="D57" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>5.44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>226</v>
       </c>
@@ -2393,8 +2574,11 @@
       <c r="D58" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>8.58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>230</v>
       </c>
@@ -2407,8 +2591,11 @@
       <c r="D59" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>234</v>
       </c>
@@ -2421,8 +2608,11 @@
       <c r="D60" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>6.18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>238</v>
       </c>
@@ -2435,8 +2625,11 @@
       <c r="D61" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>9.92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>242</v>
       </c>
@@ -2449,8 +2642,11 @@
       <c r="D62" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>6.32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>246</v>
       </c>
@@ -2463,8 +2659,11 @@
       <c r="D63" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>3.13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>250</v>
       </c>
@@ -2477,8 +2676,11 @@
       <c r="D64" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>254</v>
       </c>
@@ -2491,8 +2693,11 @@
       <c r="D65" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>258</v>
       </c>
@@ -2505,8 +2710,11 @@
       <c r="D66" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>262</v>
       </c>
@@ -2519,8 +2727,11 @@
       <c r="D67" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>6.94</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>266</v>
       </c>
@@ -2533,8 +2744,11 @@
       <c r="D68" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <v>6.12</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>270</v>
       </c>
@@ -2547,8 +2761,11 @@
       <c r="D69" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>3.27</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>274</v>
       </c>
@@ -2561,8 +2778,11 @@
       <c r="D70" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>9.6199999999999992</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>278</v>
       </c>
@@ -2575,8 +2795,11 @@
       <c r="D71" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>282</v>
       </c>
@@ -2589,8 +2812,11 @@
       <c r="D72" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>286</v>
       </c>
@@ -2603,8 +2829,11 @@
       <c r="D73" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <v>4.5599999999999996</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>290</v>
       </c>
@@ -2617,8 +2846,11 @@
       <c r="D74" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74">
+        <v>8.18</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>294</v>
       </c>
@@ -2631,8 +2863,11 @@
       <c r="D75" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <v>9.91</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>298</v>
       </c>
@@ -2645,8 +2880,11 @@
       <c r="D76" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>4.57</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>302</v>
       </c>
@@ -2659,8 +2897,11 @@
       <c r="D77" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>5.62</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>306</v>
       </c>
@@ -2673,8 +2914,11 @@
       <c r="D78" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>310</v>
       </c>
@@ -2687,8 +2931,11 @@
       <c r="D79" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <v>7.47</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>314</v>
       </c>
@@ -2701,8 +2948,11 @@
       <c r="D80" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>7.35</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>318</v>
       </c>
@@ -2715,8 +2965,11 @@
       <c r="D81" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>322</v>
       </c>
@@ -2729,8 +2982,11 @@
       <c r="D82" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <v>4.1900000000000004</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>326</v>
       </c>
@@ -2743,8 +2999,11 @@
       <c r="D83" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>330</v>
       </c>
@@ -2757,8 +3016,11 @@
       <c r="D84" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>8.9700000000000006</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>334</v>
       </c>
@@ -2771,8 +3033,11 @@
       <c r="D85" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>6.22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>338</v>
       </c>
@@ -2785,8 +3050,11 @@
       <c r="D86" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <v>9.94</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>342</v>
       </c>
@@ -2799,8 +3067,11 @@
       <c r="D87" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>346</v>
       </c>
@@ -2813,8 +3084,11 @@
       <c r="D88" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>350</v>
       </c>
@@ -2827,8 +3101,11 @@
       <c r="D89" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>354</v>
       </c>
@@ -2841,8 +3118,11 @@
       <c r="D90" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>358</v>
       </c>
@@ -2855,8 +3135,11 @@
       <c r="D91" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91">
+        <v>3.08</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>362</v>
       </c>
@@ -2869,8 +3152,11 @@
       <c r="D92" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>366</v>
       </c>
@@ -2883,8 +3169,11 @@
       <c r="D93" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93">
+        <v>7.56</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>370</v>
       </c>
@@ -2897,8 +3186,11 @@
       <c r="D94" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94">
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>374</v>
       </c>
@@ -2911,8 +3203,11 @@
       <c r="D95" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>377</v>
       </c>
@@ -2925,8 +3220,11 @@
       <c r="D96" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>381</v>
       </c>
@@ -2939,8 +3237,11 @@
       <c r="D97" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97">
+        <v>5.93</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>385</v>
       </c>
@@ -2953,8 +3254,11 @@
       <c r="D98" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>389</v>
       </c>
@@ -2967,8 +3271,11 @@
       <c r="D99" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99">
+        <v>7.41</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>393</v>
       </c>
@@ -2981,8 +3288,11 @@
       <c r="D100" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100">
+        <v>7.92</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>397</v>
       </c>
@@ -2995,8 +3305,11 @@
       <c r="D101" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101">
+        <v>6.63</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>401</v>
       </c>
@@ -3008,6 +3321,9 @@
       </c>
       <c r="D102" t="s">
         <v>404</v>
+      </c>
+      <c r="E102">
+        <v>2.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>